<commit_message>
exp 5 in progres
</commit_message>
<xml_diff>
--- a/results/resultados_exp3.xlsx
+++ b/results/resultados_exp3.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DaniR\Desktop\mng\results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15465" windowHeight="4905"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>r2</t>
   </si>
@@ -52,6 +57,15 @@
   </si>
   <si>
     <t>TODAS SEMANAS</t>
+  </si>
+  <si>
+    <t>1ª experimento</t>
+  </si>
+  <si>
+    <t>2ª experimento</t>
+  </si>
+  <si>
+    <t>3ª experimento</t>
   </si>
 </sst>
 </file>
@@ -73,7 +87,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,6 +106,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -105,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -115,9 +135,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,7 +411,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -398,14 +419,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.42578125" customWidth="1"/>
   </cols>
@@ -460,7 +482,7 @@
       <c r="C3">
         <v>0.94418201980869598</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="8">
         <v>0.95639220199999997</v>
       </c>
       <c r="E3">
@@ -477,6 +499,9 @@
       </c>
       <c r="I3">
         <v>0.94808469714238897</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="O3" s="5"/>
     </row>
@@ -490,7 +515,7 @@
       <c r="C4">
         <v>11.471117499931999</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="8">
         <v>10.082031089999999</v>
       </c>
       <c r="E4">
@@ -508,54 +533,138 @@
       <c r="I4">
         <v>10.421474586614201</v>
       </c>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0.91167113849941195</v>
+      </c>
+      <c r="C5">
+        <v>0.93803704938703802</v>
+      </c>
+      <c r="D5">
+        <v>0.92883350382173002</v>
+      </c>
+      <c r="E5">
+        <v>0.95429426727868605</v>
+      </c>
+      <c r="F5">
+        <v>0.92328851443451998</v>
+      </c>
+      <c r="G5">
+        <v>0.94795127074780206</v>
+      </c>
+      <c r="H5">
+        <v>0.93857504130979297</v>
+      </c>
+      <c r="I5">
+        <v>0.94843388394102501</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>14.2804576517137</v>
+      </c>
+      <c r="C6">
+        <v>12.0166613118024</v>
+      </c>
+      <c r="D6">
+        <v>12.629374525978299</v>
+      </c>
+      <c r="E6">
+        <v>10.1819361319198</v>
+      </c>
+      <c r="F6">
+        <v>13.0732075533873</v>
+      </c>
+      <c r="G6">
+        <v>10.6731507647791</v>
+      </c>
+      <c r="H6">
+        <v>11.915375149213</v>
+      </c>
+      <c r="I6">
+        <v>10.5092446219446</v>
+      </c>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.92117725100000003</v>
+      </c>
+      <c r="C7">
+        <v>0.94314024330771196</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.93776639791434102</v>
+      </c>
+      <c r="E7">
+        <v>0.94306344867083602</v>
+      </c>
+      <c r="F7">
+        <v>0.93247750950416497</v>
+      </c>
+      <c r="G7">
+        <v>0.93229675855294403</v>
+      </c>
+      <c r="H7">
+        <v>0.93698167900271501</v>
+      </c>
+      <c r="I7">
+        <v>0.94270560075682597</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3">
+        <v>13.198085470000001</v>
+      </c>
+      <c r="C8">
+        <v>11.039499556534</v>
+      </c>
+      <c r="D8" s="3">
+        <v>12.511352069990901</v>
+      </c>
+      <c r="E8">
+        <v>11.413477143250001</v>
+      </c>
+      <c r="F8">
+        <v>11.9832204216692</v>
+      </c>
+      <c r="G8">
+        <v>12.0533070569522</v>
+      </c>
+      <c r="H8">
+        <v>11.698344226652701</v>
+      </c>
+      <c r="I8">
+        <v>11.426105504771799</v>
+      </c>
+      <c r="J8" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J7:J8"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>